<commit_message>
Add Member From Admin Panel Fixed
</commit_message>
<xml_diff>
--- a/CRM system/Reports/UsersReport.xlsx
+++ b/CRM system/Reports/UsersReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>User ID</t>
   </si>
@@ -83,55 +83,58 @@
     <t>2024-12-05 12:29:04</t>
   </si>
   <si>
+    <t>2024-12-09 01:54:45</t>
+  </si>
+  <si>
+    <t>Test Account</t>
+  </si>
+  <si>
+    <t>test@together.com</t>
+  </si>
+  <si>
+    <t>07/06/2001</t>
+  </si>
+  <si>
+    <t>Sfsaf</t>
+  </si>
+  <si>
+    <t>2024-12-05 19:27:54</t>
+  </si>
+  <si>
+    <t>80.0%</t>
+  </si>
+  <si>
+    <t>Mike Tyson</t>
+  </si>
+  <si>
+    <t>mike@example.com</t>
+  </si>
+  <si>
+    <t>16/02/2000</t>
+  </si>
+  <si>
+    <t>2024-12-05 19:41:47</t>
+  </si>
+  <si>
+    <t>New User</t>
+  </si>
+  <si>
+    <t>new@user.com</t>
+  </si>
+  <si>
+    <t>01/08/1999</t>
+  </si>
+  <si>
+    <t>2024-12-07 17:35:04</t>
+  </si>
+  <si>
     <t>0.0%</t>
   </si>
   <si>
-    <t>Test Account</t>
-  </si>
-  <si>
-    <t>test@together.com</t>
-  </si>
-  <si>
-    <t>07/06/2001</t>
-  </si>
-  <si>
-    <t>Sfsaf</t>
-  </si>
-  <si>
-    <t>2024-12-05 19:27:54</t>
-  </si>
-  <si>
-    <t>80.0%</t>
-  </si>
-  <si>
-    <t>Mike Tyson</t>
-  </si>
-  <si>
-    <t>mike@example.com</t>
-  </si>
-  <si>
-    <t>16/02/2000</t>
-  </si>
-  <si>
-    <t>2024-12-05 19:41:47</t>
-  </si>
-  <si>
-    <t>New User</t>
-  </si>
-  <si>
-    <t>new@user.com</t>
-  </si>
-  <si>
-    <t>01/08/1999</t>
-  </si>
-  <si>
-    <t>2024-12-07 17:35:04</t>
-  </si>
-  <si>
-    <t>Tyra</t>
-  </si>
-  <si>
-    <t>tyr@tyr.com</t>
+    <t>New Form</t>
+  </si>
+  <si>
+    <t>12345@gmail.com</t>
   </si>
   <si>
     <t>pending</t>
@@ -140,13 +143,22 @@
     <t>none</t>
   </si>
   <si>
-    <t>07/12/2006</t>
-  </si>
-  <si>
-    <t>Tyr@Tyr.Com</t>
-  </si>
-  <si>
-    <t>2024-12-07 17:47:34</t>
+    <t>09/02/2000</t>
+  </si>
+  <si>
+    <t>2024-12-09 02:43:59</t>
+  </si>
+  <si>
+    <t>60.0%</t>
+  </si>
+  <si>
+    <t>Alan 2</t>
+  </si>
+  <si>
+    <t>alan2@works.com</t>
+  </si>
+  <si>
+    <t>2024-12-09 03:07:23</t>
   </si>
 </sst>
 </file>
@@ -193,7 +205,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -291,13 +303,13 @@
         <v>22</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J3" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -396,30 +408,30 @@
         <v>0</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>44</v>
@@ -428,10 +440,41 @@
         <v>44</v>
       </c>
       <c r="J7" s="0">
+        <v>3</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>17</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="0">
         <v>0</v>
       </c>
-      <c r="K7" s="0" t="s">
-        <v>23</v>
+      <c r="K8" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Admin Events Attendees page to track event attendees, remove members, and implement search functionality.
</commit_message>
<xml_diff>
--- a/CRM system/Reports/UsersReport.xlsx
+++ b/CRM system/Reports/UsersReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>User ID</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>2024-12-09 03:07:23</t>
+  </si>
+  <si>
+    <t>Alex F</t>
+  </si>
+  <si>
+    <t>alex@exmaple.come</t>
+  </si>
+  <si>
+    <t>2024-12-09 03:16:11</t>
   </si>
 </sst>
 </file>
@@ -205,7 +214,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -477,6 +486,37 @@
         <v>38</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>18</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="0">
+        <v>0</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>